<commit_message>
data & code python
</commit_message>
<xml_diff>
--- a/All-disaster.xlsx
+++ b/All-disaster.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="9">
   <si>
     <t>YEAR</t>
   </si>
@@ -44,6 +44,9 @@
   <si>
     <t>Conflagration</t>
   </si>
+  <si>
+    <t>DAMAGED</t>
+  </si>
 </sst>
 </file>
 
@@ -61,6 +64,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Comic Sans MS"/>
+      <family val="4"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -94,21 +98,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -413,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -425,9 +455,10 @@
     <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,1002 +471,1219 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="E1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>2531</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>242</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="E2" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>2532</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>5495</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>602</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="E3" s="7">
+        <v>11739.56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>2532</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>9</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="E4" s="6">
+        <v>14.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>2532</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>208</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="E5" s="6">
+        <v>671.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>2533</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>19</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="E6" s="7">
+        <v>6652.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>2533</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>118</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>126</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="E7" s="6">
+        <v>172.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>2533</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>293</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>154</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="E8" s="7">
+        <v>1490.27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>2534</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <v>26</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="E9" s="7">
+        <v>4562.3100000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>2534</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <v>55</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="E10" s="6">
+        <v>75.849999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>2534</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>168</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="E11" s="7">
+        <v>2127.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>2535</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>0</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="E12" s="7">
+        <v>5240.58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>2535</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>50</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="E13" s="6">
+        <v>193.06</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>2535</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <v>138</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="4">
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="E14" s="7">
+        <v>1094.21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>2536</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <v>254</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="E15" s="7">
+        <v>2181.61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>2536</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <v>31</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="E16" s="6">
+        <v>204.43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>2536</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <v>833</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="4">
         <v>270</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="E17" s="7">
+        <v>1751.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <v>2537</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="4">
         <v>12</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="4">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="E18" s="7">
+        <v>5058.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>2537</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="4">
         <v>46</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="E19" s="6">
+        <v>120.28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>2537</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="4">
         <v>147</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="4">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="E20" s="6">
+        <v>711.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>2538</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="4">
         <v>11</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="4">
         <v>442</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="E21" s="7">
+        <v>6123.52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>2538</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="4">
         <v>51</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="E22" s="6">
+        <v>100.41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>2538</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="4">
         <v>153</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="4">
         <v>79</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="E23" s="7">
+        <v>3038.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
         <v>2539</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="4">
         <v>21</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="4">
         <v>158</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="E24" s="7">
+        <v>7160.68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>2539</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="4">
         <v>42</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="4">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="E25" s="6">
+        <v>335.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>2539</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="4">
         <v>155</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="4">
         <v>105</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="E26" s="7">
+        <v>2528.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>2540</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="4">
         <v>427</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="4">
         <v>98</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="E27" s="7">
+        <v>3842.22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
         <v>2540</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="4">
         <v>66</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="4">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+      <c r="E28" s="6">
+        <v>518.64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
         <v>2540</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="4">
         <v>261</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="4">
         <v>217</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="E29" s="7">
+        <v>2340.96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>2541</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="4">
         <v>3</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+      <c r="E30" s="7">
+        <v>1706.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
         <v>2541</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="4">
         <v>70</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="4">
         <v>90</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+      <c r="E31" s="6">
+        <v>371.44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>2541</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="4">
         <v>100</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="4">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+      <c r="E32" s="7">
+        <v>2347.61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
         <v>2542</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="4">
         <v>30</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+      <c r="E33" s="7">
+        <v>1381.64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <v>2542</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="4">
         <v>55</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="4">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+      <c r="E34" s="6">
+        <v>192.22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
         <v>2542</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="4">
         <v>0</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="4">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="E35" s="6">
+        <v>544.51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
         <v>2543</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="4">
         <v>0</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="4">
         <v>120</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+      <c r="E36" s="7">
+        <v>10032.94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
         <v>2543</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="4">
         <v>81</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="E37" s="6">
+        <v>271.48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
         <v>2543</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="4">
         <v>91</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="4">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+      <c r="E38" s="7">
+        <v>1250.6500000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>2543</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="4">
         <v>0</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+      <c r="E39" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
         <v>2544</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="4">
         <v>68</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="4">
         <v>244</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
+      <c r="E40" s="7">
+        <v>3666.29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
         <v>2544</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="4">
         <v>19</v>
       </c>
-      <c r="D41" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
+      <c r="D41" s="4">
+        <v>6</v>
+      </c>
+      <c r="E41" s="6">
+        <v>501.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <v>2544</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="4">
         <v>148</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
+      <c r="E42" s="7">
+        <v>1529.28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <v>2544</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="4">
         <v>109</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="4">
         <v>136</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+      <c r="E43" s="6">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
         <v>2545</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="4">
         <v>0</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="4">
         <v>216</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+      <c r="E44" s="7">
+        <v>13385.32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <v>2545</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="4">
         <v>11</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+      <c r="E45" s="6">
+        <v>213.34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
         <v>2545</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="4">
         <v>150</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="4">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
+      <c r="E46" s="6">
+        <v>805.81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
         <v>2546</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="4">
         <v>10</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="4">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
+      <c r="E47" s="7">
+        <v>2050.2600000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
         <v>2546</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="4">
         <v>434</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="4">
         <v>74</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+      <c r="E48" s="6">
+        <v>457.43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
         <v>2546</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="4">
         <v>167</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="4">
         <v>56</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+      <c r="E49" s="6">
+        <v>565.54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
         <v>2547</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="4">
         <v>3</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="4">
         <v>28</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
+      <c r="E50" s="6">
+        <v>850.65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
         <v>2547</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="4">
         <v>63</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="4">
         <v>73</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
+      <c r="E51" s="6">
+        <v>398.41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
         <v>2547</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="4">
         <v>69</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="4">
         <v>31</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
+      <c r="E52" s="6">
+        <v>487.02</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
         <v>2547</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="4">
         <v>391</v>
       </c>
-      <c r="D53" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
+      <c r="D53" s="4">
+        <v>5</v>
+      </c>
+      <c r="E53" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
         <v>2548</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="4">
         <v>0</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="4">
         <v>75</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
+      <c r="E54" s="7">
+        <v>5982.28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
         <v>2548</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="4">
         <v>0</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
+      <c r="E55" s="6">
+        <v>148.87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
         <v>2548</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="4">
         <v>68</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="4">
         <v>48</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
+      <c r="E56" s="6">
+        <v>931.91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
         <v>2549</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="4">
         <v>1462</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="4">
         <v>446</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
+      <c r="E57" s="7">
+        <v>9627.41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
         <v>2549</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="4">
         <v>39</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="4">
         <v>29</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
+      <c r="E58" s="6">
+        <v>92.24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
         <v>2549</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="4">
         <v>66</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="4">
         <v>37</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
+      <c r="E59" s="7">
+        <v>1083.8399999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
         <v>2549</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="4">
         <v>0</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="4">
         <v>83</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
+      <c r="E60" s="4">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
         <v>2550</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="4">
         <v>17</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="4">
         <v>36</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
+      <c r="E61" s="7">
+        <v>1687.86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
         <v>2550</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="4">
         <v>71</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
+      <c r="E62" s="6">
+        <v>234.54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
         <v>2550</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="4">
         <v>156</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
+      <c r="E63" s="6">
+        <v>875.79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
         <v>2550</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="4">
         <v>0</v>
       </c>
-      <c r="D64" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
+      <c r="D64" s="4">
+        <v>6</v>
+      </c>
+      <c r="E64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
         <v>2551</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="4">
         <v>16</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="4">
         <v>113</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
+      <c r="E65" s="7">
+        <v>7601.79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
         <v>2551</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="4">
         <v>30</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
+      <c r="E66" s="6">
+        <v>227.54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
         <v>2551</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="4">
         <v>92</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
+      <c r="E67" s="7">
+        <v>1424.89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
         <v>2551</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="4">
         <v>0</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
+      <c r="E68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
         <v>2552</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="4">
         <v>22</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
+      <c r="E69" s="7">
+        <v>5252.61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
         <v>2552</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="4">
         <v>26</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="4">
         <v>24</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
+      <c r="E70" s="6">
+        <v>207.37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
         <v>2552</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="4">
         <v>312</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="4">
         <v>83</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
+      <c r="E71" s="6">
+        <v>817.33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
         <v>2552</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="4">
         <v>0</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="4">
         <v>14</v>
+      </c>
+      <c r="E72" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>